<commit_message>
bug fix, repeat data
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -408,7 +408,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H2" t="str">
-        <v>8d17b769</v>
+        <v>af099477</v>
       </c>
     </row>
     <row r="3">
@@ -428,7 +428,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H3" t="str">
-        <v>24829de7</v>
+        <v>796b1430</v>
       </c>
     </row>
     <row r="4">
@@ -448,7 +448,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H4" t="str">
-        <v>90eea3e0</v>
+        <v>ba4ff582</v>
       </c>
     </row>
     <row r="5">
@@ -468,7 +468,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H5" t="str">
-        <v>6f2690d0</v>
+        <v>12e20d5e</v>
       </c>
     </row>
     <row r="6">
@@ -488,7 +488,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H6" t="str">
-        <v>3e9225eb</v>
+        <v>0c598d6b</v>
       </c>
     </row>
     <row r="7">
@@ -508,7 +508,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H7" t="str">
-        <v>c9714ff9</v>
+        <v>f22692e3</v>
       </c>
     </row>
     <row r="8">
@@ -528,7 +528,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H8" t="str">
-        <v>2b824983</v>
+        <v>1d8d0241</v>
       </c>
     </row>
     <row r="9">
@@ -548,7 +548,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H9" t="str">
-        <v>4f36369a</v>
+        <v>392a0e3d</v>
       </c>
     </row>
     <row r="10">
@@ -568,7 +568,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H10" t="str">
-        <v>4ffde464</v>
+        <v>c15ca7d4</v>
       </c>
     </row>
     <row r="11">
@@ -588,7 +588,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H11" t="str">
-        <v>e525b96d</v>
+        <v>488c02a5</v>
       </c>
     </row>
     <row r="12">
@@ -608,7 +608,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H12" t="str">
-        <v>6f40e9c6</v>
+        <v>5fd47653</v>
       </c>
     </row>
     <row r="13">
@@ -628,7 +628,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H13" t="str">
-        <v>cc646a18</v>
+        <v>187c5194</v>
       </c>
     </row>
     <row r="14">
@@ -648,7 +648,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H14" t="str">
-        <v>b3d2e1dd</v>
+        <v>1927ce30</v>
       </c>
     </row>
     <row r="15">
@@ -668,7 +668,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H15" t="str">
-        <v>6b74c6e6</v>
+        <v>b7283f31</v>
       </c>
     </row>
     <row r="16">
@@ -688,7 +688,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H16" t="str">
-        <v>65cfde1e</v>
+        <v>5c56eefb</v>
       </c>
     </row>
     <row r="17">
@@ -708,7 +708,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H17" t="str">
-        <v>fd330e3e</v>
+        <v>ebbf7b2a</v>
       </c>
     </row>
     <row r="18">
@@ -728,7 +728,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H18" t="str">
-        <v>f6a2a7e4</v>
+        <v>928ac21f</v>
       </c>
     </row>
     <row r="19">
@@ -748,7 +748,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H19" t="str">
-        <v>70e9bfa4</v>
+        <v>7ad7542c</v>
       </c>
     </row>
     <row r="20">
@@ -768,7 +768,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H20" t="str">
-        <v>1d8e4595</v>
+        <v>46f8fb0b</v>
       </c>
     </row>
     <row r="21">
@@ -788,7 +788,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H21" t="str">
-        <v>d6831f3f</v>
+        <v>664ccb63</v>
       </c>
     </row>
     <row r="22">
@@ -808,7 +808,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H22" t="str">
-        <v>5570e46c</v>
+        <v>a446b23e</v>
       </c>
     </row>
     <row r="23">
@@ -828,7 +828,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H23" t="str">
-        <v>50bb32bf</v>
+        <v>1dc9b702</v>
       </c>
     </row>
     <row r="24">
@@ -848,7 +848,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H24" t="str">
-        <v>f31b2e80</v>
+        <v>f2fd5b6e</v>
       </c>
     </row>
     <row r="25">
@@ -868,7 +868,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H25" t="str">
-        <v>229ecfce</v>
+        <v>c90245c2</v>
       </c>
     </row>
     <row r="26">
@@ -888,7 +888,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H26" t="str">
-        <v>7cc00c3e</v>
+        <v>8914aae6</v>
       </c>
     </row>
     <row r="27">
@@ -908,7 +908,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H27" t="str">
-        <v>ebc0109d</v>
+        <v>3d3dd3ab</v>
       </c>
     </row>
     <row r="28">
@@ -928,7 +928,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H28" t="str">
-        <v>9d2e7e8d</v>
+        <v>eea57c5f</v>
       </c>
     </row>
     <row r="29">
@@ -948,7 +948,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H29" t="str">
-        <v>02f01563</v>
+        <v>4b8c6408</v>
       </c>
     </row>
     <row r="30">
@@ -968,7 +968,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H30" t="str">
-        <v>e7e8e229</v>
+        <v>28549724</v>
       </c>
     </row>
     <row r="31">
@@ -988,7 +988,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H31" t="str">
-        <v>aec22f0a</v>
+        <v>bc0882ce</v>
       </c>
     </row>
     <row r="32">
@@ -1008,7 +1008,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H32" t="str">
-        <v>1fe37c13</v>
+        <v>938666fc</v>
       </c>
     </row>
     <row r="33">
@@ -1028,7 +1028,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H33" t="str">
-        <v>ab34219d</v>
+        <v>9a3dcafe</v>
       </c>
     </row>
     <row r="34">
@@ -1048,7 +1048,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H34" t="str">
-        <v>b30e1fb0</v>
+        <v>c8e0b309</v>
       </c>
     </row>
     <row r="35">
@@ -1068,7 +1068,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H35" t="str">
-        <v>3cbaadd8</v>
+        <v>e37c80f7</v>
       </c>
     </row>
     <row r="36">
@@ -1088,7 +1088,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H36" t="str">
-        <v>82964ba7</v>
+        <v>9ab4083b</v>
       </c>
     </row>
     <row r="37">
@@ -1108,7 +1108,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H37" t="str">
-        <v>96961bbf</v>
+        <v>9deb5ab1</v>
       </c>
     </row>
     <row r="38">
@@ -1128,7 +1128,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H38" t="str">
-        <v>183c3e0b</v>
+        <v>82f8e773</v>
       </c>
     </row>
     <row r="39">
@@ -1148,7 +1148,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H39" t="str">
-        <v>ebfef966</v>
+        <v>1deb67e5</v>
       </c>
     </row>
     <row r="40">
@@ -1168,7 +1168,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H40" t="str">
-        <v>f6dda408</v>
+        <v>1fe587bc</v>
       </c>
     </row>
     <row r="41">
@@ -1188,7 +1188,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H41" t="str">
-        <v>77579898</v>
+        <v>35be32d9</v>
       </c>
     </row>
     <row r="42">
@@ -1208,7 +1208,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H42" t="str">
-        <v>f2a05a23</v>
+        <v>ae408afd</v>
       </c>
     </row>
     <row r="43">
@@ -1228,7 +1228,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H43" t="str">
-        <v>cca5a896</v>
+        <v>4b455c44</v>
       </c>
     </row>
     <row r="44">
@@ -1248,7 +1248,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H44" t="str">
-        <v>3241ba84</v>
+        <v>15085f8b</v>
       </c>
     </row>
     <row r="45">
@@ -1268,7 +1268,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H45" t="str">
-        <v>eb3226cd</v>
+        <v>d302d766</v>
       </c>
     </row>
     <row r="46">
@@ -1288,7 +1288,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H46" t="str">
-        <v>9f5d24a9</v>
+        <v>7085db31</v>
       </c>
     </row>
     <row r="47">
@@ -1308,7 +1308,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H47" t="str">
-        <v>2ca7fbcd</v>
+        <v>e5070495</v>
       </c>
     </row>
     <row r="48">
@@ -1328,7 +1328,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H48" t="str">
-        <v>04cfe122</v>
+        <v>87db26a4</v>
       </c>
     </row>
     <row r="49">
@@ -1348,7 +1348,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H49" t="str">
-        <v>0521e4c1</v>
+        <v>fb3d146b</v>
       </c>
     </row>
     <row r="50">
@@ -1368,7 +1368,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H50" t="str">
-        <v>717862d8</v>
+        <v>67572119</v>
       </c>
     </row>
     <row r="51">
@@ -1388,7 +1388,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H51" t="str">
-        <v>4df90b18</v>
+        <v>dc88cc5f</v>
       </c>
     </row>
     <row r="52">
@@ -1408,7 +1408,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H52" t="str">
-        <v>a5cc5991</v>
+        <v>b7098070</v>
       </c>
     </row>
     <row r="53">
@@ -1428,7 +1428,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H53" t="str">
-        <v>a63ae929</v>
+        <v>450bfd1b</v>
       </c>
     </row>
     <row r="54">
@@ -1448,7 +1448,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H54" t="str">
-        <v>079bbd60</v>
+        <v>d5bc3d50</v>
       </c>
     </row>
     <row r="55">
@@ -1468,7 +1468,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H55" t="str">
-        <v>7b21a1b0</v>
+        <v>e5087ac3</v>
       </c>
     </row>
     <row r="56">
@@ -1488,7 +1488,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H56" t="str">
-        <v>d5746857</v>
+        <v>6c56b9e2</v>
       </c>
     </row>
     <row r="57">
@@ -1508,7 +1508,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H57" t="str">
-        <v>53acd6bc</v>
+        <v>747c9a85</v>
       </c>
     </row>
     <row r="58">
@@ -1528,7 +1528,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H58" t="str">
-        <v>ac7f7878</v>
+        <v>8cfe7b61</v>
       </c>
     </row>
     <row r="59">
@@ -1548,7 +1548,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H59" t="str">
-        <v>3e6cee32</v>
+        <v>3eec2589</v>
       </c>
     </row>
     <row r="60">
@@ -1568,7 +1568,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H60" t="str">
-        <v>a823ebc0</v>
+        <v>4bc73ffc</v>
       </c>
     </row>
     <row r="61">
@@ -1588,7 +1588,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H61" t="str">
-        <v>aca6cb06</v>
+        <v>6d60c487</v>
       </c>
     </row>
     <row r="62">
@@ -1608,7 +1608,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H62" t="str">
-        <v>c07c1845</v>
+        <v>2c2da532</v>
       </c>
     </row>
     <row r="63">
@@ -1628,7 +1628,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H63" t="str">
-        <v>94dc2d22</v>
+        <v>f2d46318</v>
       </c>
     </row>
     <row r="64">
@@ -1648,7 +1648,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H64" t="str">
-        <v>1ffdc7be</v>
+        <v>e675999f</v>
       </c>
     </row>
     <row r="65">
@@ -1668,7 +1668,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H65" t="str">
-        <v>68d16342</v>
+        <v>eb19cb7f</v>
       </c>
     </row>
     <row r="66">
@@ -1688,7 +1688,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H66" t="str">
-        <v>c8ae7ec0</v>
+        <v>f57c282c</v>
       </c>
     </row>
     <row r="67">
@@ -1708,7 +1708,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H67" t="str">
-        <v>17db686d</v>
+        <v>0da45e8e</v>
       </c>
     </row>
     <row r="68">
@@ -1728,7 +1728,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H68" t="str">
-        <v>cb98da8c</v>
+        <v>637da438</v>
       </c>
     </row>
     <row r="69">
@@ -1748,7 +1748,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H69" t="str">
-        <v>6fa2656d</v>
+        <v>08a5044f</v>
       </c>
     </row>
     <row r="70">
@@ -1768,7 +1768,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H70" t="str">
-        <v>d9d03f8f</v>
+        <v>959e20b7</v>
       </c>
     </row>
     <row r="71">
@@ -1788,7 +1788,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H71" t="str">
-        <v>dc3539d9</v>
+        <v>36a2ce83</v>
       </c>
     </row>
     <row r="72">
@@ -1808,7 +1808,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H72" t="str">
-        <v>80608ea5</v>
+        <v>97458f0b</v>
       </c>
     </row>
     <row r="73">
@@ -1828,7 +1828,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H73" t="str">
-        <v>67c87514</v>
+        <v>6e9bb971</v>
       </c>
     </row>
     <row r="74">
@@ -1848,7 +1848,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H74" t="str">
-        <v>5508b553</v>
+        <v>34c546ef</v>
       </c>
     </row>
     <row r="75">
@@ -1868,7 +1868,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H75" t="str">
-        <v>4ab38104</v>
+        <v>27b9f171</v>
       </c>
     </row>
     <row r="76">
@@ -1888,7 +1888,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H76" t="str">
-        <v>db9ef725</v>
+        <v>cd05bdf7</v>
       </c>
     </row>
     <row r="77">
@@ -1908,7 +1908,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H77" t="str">
-        <v>91b3d059</v>
+        <v>97564e91</v>
       </c>
     </row>
     <row r="78">
@@ -1928,7 +1928,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H78" t="str">
-        <v>99664506</v>
+        <v>f781b33d</v>
       </c>
     </row>
     <row r="79">
@@ -1948,7 +1948,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H79" t="str">
-        <v>291c1443</v>
+        <v>beae618b</v>
       </c>
     </row>
     <row r="80">
@@ -1968,7 +1968,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H80" t="str">
-        <v>aa7daa52</v>
+        <v>e693cedd</v>
       </c>
     </row>
     <row r="81">
@@ -1988,7 +1988,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H81" t="str">
-        <v>ca9df21a</v>
+        <v>6665fb64</v>
       </c>
     </row>
     <row r="82">
@@ -2008,7 +2008,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H82" t="str">
-        <v>711f7c77</v>
+        <v>7ae07745</v>
       </c>
     </row>
     <row r="83">
@@ -2028,7 +2028,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H83" t="str">
-        <v>c41c2b05</v>
+        <v>944063ff</v>
       </c>
     </row>
     <row r="84">
@@ -2048,7 +2048,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H84" t="str">
-        <v>77f7d438</v>
+        <v>31b078a3</v>
       </c>
     </row>
     <row r="85">
@@ -2068,7 +2068,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H85" t="str">
-        <v>5403aa6b</v>
+        <v>c9a67e76</v>
       </c>
     </row>
     <row r="86">
@@ -2088,7 +2088,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H86" t="str">
-        <v>401c4817</v>
+        <v>4c136138</v>
       </c>
     </row>
     <row r="87">
@@ -2108,7 +2108,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H87" t="str">
-        <v>48bc7271</v>
+        <v>9e09963c</v>
       </c>
     </row>
     <row r="88">
@@ -2128,7 +2128,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H88" t="str">
-        <v>50eedafc</v>
+        <v>e2060487</v>
       </c>
     </row>
     <row r="89">
@@ -2148,7 +2148,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H89" t="str">
-        <v>e21d26d1</v>
+        <v>c5fa59ef</v>
       </c>
     </row>
     <row r="90">
@@ -2168,7 +2168,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H90" t="str">
-        <v>24993800</v>
+        <v>e1080f0c</v>
       </c>
     </row>
     <row r="91">
@@ -2188,7 +2188,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H91" t="str">
-        <v>8a203289</v>
+        <v>2e3343bf</v>
       </c>
     </row>
     <row r="92">
@@ -2208,7 +2208,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H92" t="str">
-        <v>7ba4792a</v>
+        <v>39fae90a</v>
       </c>
     </row>
     <row r="93">
@@ -2228,7 +2228,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H93" t="str">
-        <v>72fb5ffd</v>
+        <v>bd536f06</v>
       </c>
     </row>
     <row r="94">
@@ -2248,7 +2248,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H94" t="str">
-        <v>3a567d2e</v>
+        <v>7c21b67b</v>
       </c>
     </row>
     <row r="95">
@@ -2268,7 +2268,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H95" t="str">
-        <v>8441368c</v>
+        <v>92de3996</v>
       </c>
     </row>
     <row r="96">
@@ -2288,7 +2288,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H96" t="str">
-        <v>fe723804</v>
+        <v>8c4d5cc2</v>
       </c>
     </row>
     <row r="97">
@@ -2308,7 +2308,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H97" t="str">
-        <v>90c46085</v>
+        <v>fbf7fb2a</v>
       </c>
     </row>
     <row r="98">
@@ -2328,7 +2328,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H98" t="str">
-        <v>4624e8f2</v>
+        <v>7b95754f</v>
       </c>
     </row>
     <row r="99">
@@ -2348,7 +2348,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H99" t="str">
-        <v>454885ea</v>
+        <v>882cdd10</v>
       </c>
     </row>
     <row r="100">
@@ -2368,7 +2368,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H100" t="str">
-        <v>2db4bc4b</v>
+        <v>7a3f0ea4</v>
       </c>
     </row>
     <row r="101">
@@ -2388,7 +2388,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H101" t="str">
-        <v>7f3463e0</v>
+        <v>25d64b37</v>
       </c>
     </row>
     <row r="102">
@@ -2408,7 +2408,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H102" t="str">
-        <v>4416dd66</v>
+        <v>80b10a49</v>
       </c>
     </row>
     <row r="103">
@@ -2428,7 +2428,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H103" t="str">
-        <v>1675f073</v>
+        <v>7c5f4eb7</v>
       </c>
     </row>
     <row r="104">
@@ -2448,7 +2448,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H104" t="str">
-        <v>f4c0e440</v>
+        <v>47f1dcc5</v>
       </c>
     </row>
     <row r="105">
@@ -2468,7 +2468,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H105" t="str">
-        <v>b86dfbd6</v>
+        <v>52ac0bea</v>
       </c>
     </row>
     <row r="106">
@@ -2488,7 +2488,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H106" t="str">
-        <v>011d34a9</v>
+        <v>23dddf3b</v>
       </c>
     </row>
     <row r="107">
@@ -2508,7 +2508,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H107" t="str">
-        <v>b1df8427</v>
+        <v>653a85e3</v>
       </c>
     </row>
     <row r="108">
@@ -2528,7 +2528,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H108" t="str">
-        <v>6acd57d7</v>
+        <v>d83c746a</v>
       </c>
     </row>
     <row r="109">
@@ -2548,7 +2548,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H109" t="str">
-        <v>f966baa6</v>
+        <v>09e0b99e</v>
       </c>
     </row>
     <row r="110">
@@ -2568,7 +2568,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H110" t="str">
-        <v>4cde8baf</v>
+        <v>b775e52b</v>
       </c>
     </row>
     <row r="111">
@@ -2588,7 +2588,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H111" t="str">
-        <v>25b76a74</v>
+        <v>3f4467fe</v>
       </c>
     </row>
     <row r="112">
@@ -2608,7 +2608,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H112" t="str">
-        <v>80b76988</v>
+        <v>1a1f15e9</v>
       </c>
     </row>
     <row r="113">
@@ -2628,7 +2628,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H113" t="str">
-        <v>1a84957f</v>
+        <v>6b99e58e</v>
       </c>
     </row>
     <row r="114">
@@ -2648,7 +2648,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H114" t="str">
-        <v>4e9eda41</v>
+        <v>07a32b42</v>
       </c>
     </row>
     <row r="115">
@@ -2668,7 +2668,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H115" t="str">
-        <v>f8768cc3</v>
+        <v>7ab011af</v>
       </c>
     </row>
     <row r="116">
@@ -2688,7 +2688,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H116" t="str">
-        <v>0d42278d</v>
+        <v>258dee81</v>
       </c>
     </row>
     <row r="117">
@@ -2708,7 +2708,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H117" t="str">
-        <v>6ee73679</v>
+        <v>753311bb</v>
       </c>
     </row>
     <row r="118">
@@ -2728,7 +2728,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H118" t="str">
-        <v>927f2d79</v>
+        <v>2a5c516a</v>
       </c>
     </row>
     <row r="119">
@@ -2748,7 +2748,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H119" t="str">
-        <v>51d7e17b</v>
+        <v>b8bd88ec</v>
       </c>
     </row>
     <row r="120">
@@ -2768,7 +2768,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H120" t="str">
-        <v>ee7ba6cc</v>
+        <v>f9b94be2</v>
       </c>
     </row>
     <row r="121">
@@ -2788,7 +2788,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H121" t="str">
-        <v>72682f21</v>
+        <v>99611e23</v>
       </c>
     </row>
     <row r="122">
@@ -2808,7 +2808,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H122" t="str">
-        <v>eddd77ca</v>
+        <v>95ae58d6</v>
       </c>
     </row>
     <row r="123">
@@ -2828,7 +2828,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H123" t="str">
-        <v>d1f83463</v>
+        <v>3fb144d4</v>
       </c>
     </row>
     <row r="124">
@@ -2848,7 +2848,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H124" t="str">
-        <v>b57c26be</v>
+        <v>ef73fdbd</v>
       </c>
     </row>
     <row r="125">
@@ -2868,7 +2868,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H125" t="str">
-        <v>aaf00548</v>
+        <v>c4f65788</v>
       </c>
     </row>
     <row r="126">
@@ -2888,7 +2888,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H126" t="str">
-        <v>3fb81e3a</v>
+        <v>3f0afc92</v>
       </c>
     </row>
     <row r="127">
@@ -2908,7 +2908,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H127" t="str">
-        <v>80e066b0</v>
+        <v>341ea0b6</v>
       </c>
     </row>
     <row r="128">
@@ -2928,7 +2928,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H128" t="str">
-        <v>aa6bee94</v>
+        <v>20e24896</v>
       </c>
     </row>
     <row r="129">
@@ -2948,7 +2948,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H129" t="str">
-        <v>6dde8119</v>
+        <v>505f170f</v>
       </c>
     </row>
     <row r="130">
@@ -2968,7 +2968,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H130" t="str">
-        <v>564a3ba5</v>
+        <v>5700f1c0</v>
       </c>
     </row>
     <row r="131">
@@ -2988,7 +2988,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H131" t="str">
-        <v>4deae63c</v>
+        <v>88935779</v>
       </c>
     </row>
     <row r="132">
@@ -3008,7 +3008,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H132" t="str">
-        <v>39c0f41d</v>
+        <v>ab8aea9a</v>
       </c>
     </row>
     <row r="133">
@@ -3028,7 +3028,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H133" t="str">
-        <v>dcfb8d7b</v>
+        <v>c677f64b</v>
       </c>
     </row>
     <row r="134">
@@ -3048,7 +3048,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H134" t="str">
-        <v>06ee5ad7</v>
+        <v>2a008ef5</v>
       </c>
     </row>
     <row r="135">
@@ -3068,7 +3068,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H135" t="str">
-        <v>6e8ee685</v>
+        <v>d650f90d</v>
       </c>
     </row>
     <row r="136">
@@ -3088,7 +3088,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H136" t="str">
-        <v>ad0aff28</v>
+        <v>e4790a2b</v>
       </c>
     </row>
     <row r="137">
@@ -3108,7 +3108,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H137" t="str">
-        <v>5b095c05</v>
+        <v>991a0913</v>
       </c>
     </row>
     <row r="138">
@@ -3128,7 +3128,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H138" t="str">
-        <v>9101bc58</v>
+        <v>18cda2a7</v>
       </c>
     </row>
     <row r="139">
@@ -3148,7 +3148,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H139" t="str">
-        <v>b4dbdf95</v>
+        <v>b1ecb059</v>
       </c>
     </row>
     <row r="140">
@@ -3168,7 +3168,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H140" t="str">
-        <v>2b98fa60</v>
+        <v>2d062e97</v>
       </c>
     </row>
     <row r="141">
@@ -3188,7 +3188,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H141" t="str">
-        <v>8b3934b2</v>
+        <v>9a5ba7e5</v>
       </c>
     </row>
     <row r="142">
@@ -3208,7 +3208,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H142" t="str">
-        <v>a55f7b3e</v>
+        <v>dbe2392c</v>
       </c>
     </row>
     <row r="143">
@@ -3228,7 +3228,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H143" t="str">
-        <v>18ca68f7</v>
+        <v>c528d11b</v>
       </c>
     </row>
     <row r="144">
@@ -3248,7 +3248,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H144" t="str">
-        <v>67277a59</v>
+        <v>39d70f68</v>
       </c>
     </row>
     <row r="145">
@@ -3268,7 +3268,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H145" t="str">
-        <v>a74648c6</v>
+        <v>7e82ddbb</v>
       </c>
     </row>
     <row r="146">
@@ -3288,7 +3288,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H146" t="str">
-        <v>1e23706b</v>
+        <v>5405ec2b</v>
       </c>
     </row>
     <row r="147">
@@ -3308,7 +3308,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H147" t="str">
-        <v>170680c7</v>
+        <v>061f8e2d</v>
       </c>
     </row>
     <row r="148">
@@ -3328,7 +3328,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H148" t="str">
-        <v>ee639a54</v>
+        <v>6ed3b06a</v>
       </c>
     </row>
     <row r="149">
@@ -3348,7 +3348,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H149" t="str">
-        <v>e9ccc0e5</v>
+        <v>20fc9b38</v>
       </c>
     </row>
     <row r="150">
@@ -3368,7 +3368,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H150" t="str">
-        <v>e651999e</v>
+        <v>397ca239</v>
       </c>
     </row>
     <row r="151">
@@ -3388,7 +3388,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H151" t="str">
-        <v>705653cd</v>
+        <v>161d1790</v>
       </c>
     </row>
     <row r="152">
@@ -3408,7 +3408,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H152" t="str">
-        <v>e287f5d2</v>
+        <v>2d564643</v>
       </c>
     </row>
     <row r="153">
@@ -3428,7 +3428,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H153" t="str">
-        <v>5eb69109</v>
+        <v>5412b02d</v>
       </c>
     </row>
     <row r="154">
@@ -3448,7 +3448,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H154" t="str">
-        <v>216ad457</v>
+        <v>01def707</v>
       </c>
     </row>
     <row r="155">
@@ -3468,7 +3468,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H155" t="str">
-        <v>b584bb1e</v>
+        <v>c57295d4</v>
       </c>
     </row>
     <row r="156">
@@ -3488,7 +3488,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H156" t="str">
-        <v>2f37a8ab</v>
+        <v>d1758c47</v>
       </c>
     </row>
     <row r="157">
@@ -3508,7 +3508,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H157" t="str">
-        <v>2c5a556e</v>
+        <v>0a8efff9</v>
       </c>
     </row>
     <row r="158">
@@ -3528,7 +3528,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H158" t="str">
-        <v>eb80a458</v>
+        <v>25268b27</v>
       </c>
     </row>
     <row r="159">
@@ -3548,7 +3548,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H159" t="str">
-        <v>21d8a848</v>
+        <v>5f44bd92</v>
       </c>
     </row>
     <row r="160">
@@ -3568,7 +3568,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H160" t="str">
-        <v>a0f5f988</v>
+        <v>14b9acac</v>
       </c>
     </row>
     <row r="161">
@@ -3588,7 +3588,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H161" t="str">
-        <v>042b3dc7</v>
+        <v>b9c7cd71</v>
       </c>
     </row>
     <row r="162">
@@ -3608,7 +3608,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H162" t="str">
-        <v>a58616d7</v>
+        <v>be2132c1</v>
       </c>
     </row>
     <row r="163">
@@ -3628,7 +3628,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H163" t="str">
-        <v>0225826f</v>
+        <v>0651e938</v>
       </c>
     </row>
     <row r="164">
@@ -3648,7 +3648,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H164" t="str">
-        <v>098aaaa0</v>
+        <v>39cd66f6</v>
       </c>
     </row>
     <row r="165">
@@ -3668,7 +3668,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H165" t="str">
-        <v>f98fb847</v>
+        <v>67fb67c5</v>
       </c>
     </row>
     <row r="166">
@@ -3688,7 +3688,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H166" t="str">
-        <v>0ffe8fdb</v>
+        <v>a6fd51b1</v>
       </c>
     </row>
     <row r="167">
@@ -3708,7 +3708,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H167" t="str">
-        <v>1cde2f64</v>
+        <v>7adf94d3</v>
       </c>
     </row>
     <row r="168">
@@ -3728,7 +3728,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H168" t="str">
-        <v>3728f14c</v>
+        <v>20905e91</v>
       </c>
     </row>
     <row r="169">
@@ -3748,7 +3748,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H169" t="str">
-        <v>9d4f80b3</v>
+        <v>09aadc1c</v>
       </c>
     </row>
     <row r="170">
@@ -3768,7 +3768,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H170" t="str">
-        <v>65fa6f8f</v>
+        <v>46c36e3d</v>
       </c>
     </row>
     <row r="171">
@@ -3788,7 +3788,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H171" t="str">
-        <v>f427b862</v>
+        <v>b136b895</v>
       </c>
     </row>
     <row r="172">
@@ -3808,7 +3808,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H172" t="str">
-        <v>8c4541a4</v>
+        <v>fdb7cc62</v>
       </c>
     </row>
     <row r="173">
@@ -3828,7 +3828,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H173" t="str">
-        <v>866c192c</v>
+        <v>7e350e6f</v>
       </c>
     </row>
     <row r="174">
@@ -3848,7 +3848,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H174" t="str">
-        <v>155b7ca5</v>
+        <v>9e076cc2</v>
       </c>
     </row>
     <row r="175">
@@ -3868,7 +3868,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H175" t="str">
-        <v>f474ed03</v>
+        <v>7d239217</v>
       </c>
     </row>
     <row r="176">
@@ -3888,7 +3888,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H176" t="str">
-        <v>d5377d08</v>
+        <v>d147a1fd</v>
       </c>
     </row>
     <row r="177">
@@ -3908,7 +3908,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H177" t="str">
-        <v>e34c0411</v>
+        <v>914613c0</v>
       </c>
     </row>
     <row r="178">
@@ -3928,7 +3928,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H178" t="str">
-        <v>8457872b</v>
+        <v>e46064ea</v>
       </c>
     </row>
     <row r="179">
@@ -3948,7 +3948,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H179" t="str">
-        <v>bf12e810</v>
+        <v>45266b75</v>
       </c>
     </row>
     <row r="180">
@@ -3968,7 +3968,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H180" t="str">
-        <v>d650cbc0</v>
+        <v>880d25c7</v>
       </c>
     </row>
     <row r="181">
@@ -3988,7 +3988,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H181" t="str">
-        <v>e2b571c9</v>
+        <v>53cdbf31</v>
       </c>
     </row>
     <row r="182">
@@ -4008,7 +4008,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H182" t="str">
-        <v>3f05ed6c</v>
+        <v>4ec7ebbe</v>
       </c>
     </row>
     <row r="183">
@@ -4028,7 +4028,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H183" t="str">
-        <v>ff8a6fe1</v>
+        <v>8a54e222</v>
       </c>
     </row>
     <row r="184">
@@ -4048,7 +4048,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H184" t="str">
-        <v>f1832933</v>
+        <v>541e4454</v>
       </c>
     </row>
     <row r="185">
@@ -4068,7 +4068,7 @@
         <v>Contraseña</v>
       </c>
       <c r="H185" t="str">
-        <v>cf6785c0</v>
+        <v>a94271ef</v>
       </c>
     </row>
   </sheetData>

</xml_diff>